<commit_message>
Added *_ExternalURL for services to the scenario data. Updated CAS list logic to test for the service so that only a CAS that provides the service will appear on the list for selection.
</commit_message>
<xml_diff>
--- a/CAS_scenario.xlsx
+++ b/CAS_scenario.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="118">
   <si>
     <t>Name</t>
   </si>
@@ -314,6 +314,60 @@
   </si>
   <si>
     <t>ExternalAuthenicationMethods</t>
+  </si>
+  <si>
+    <t>https://us.mail.corp.com/owa</t>
+  </si>
+  <si>
+    <t>https://us.legacy.corp.com/owa</t>
+  </si>
+  <si>
+    <t>https://eu.mail.corp.com/owa</t>
+  </si>
+  <si>
+    <t>https://eu.legacy.corp.com/owa</t>
+  </si>
+  <si>
+    <t>https://lgb.mail.corp.com/owa</t>
+  </si>
+  <si>
+    <t>https://us.mail.corp.com/Microsoft-Server-ActiveSync</t>
+  </si>
+  <si>
+    <t>https://us.legacy.corp.com/Microsoft-Server-ActiveSync</t>
+  </si>
+  <si>
+    <t>https://eu.mail.corp.com/Microsoft-Server-ActiveSync</t>
+  </si>
+  <si>
+    <t>https://eu.legacy.corp.com/Microsoft-Server-ActiveSync</t>
+  </si>
+  <si>
+    <t>https://lgb.mail.corp.com/Microsoft-Server-ActiveSync</t>
+  </si>
+  <si>
+    <t>https://us.mail.corp.com/EWS/Exchange.asmx</t>
+  </si>
+  <si>
+    <t>https://us.legacy.corp.com/EWS/Exchange.asmx</t>
+  </si>
+  <si>
+    <t>https://eu.mail.corp.com/EWS/Exchange.asmx</t>
+  </si>
+  <si>
+    <t>https://eu.legacy.corp.com/EWS/Exchange.asmx</t>
+  </si>
+  <si>
+    <t>https://lgb.mail.corp.com/EWS/Exchange.asmx</t>
+  </si>
+  <si>
+    <t>https://us.mail.corp.com/ecp</t>
+  </si>
+  <si>
+    <t>https://eu.mail.corp.com/ecp</t>
+  </si>
+  <si>
+    <t>https://lgb.mail.corp.com/ecp</t>
   </si>
 </sst>
 </file>
@@ -1157,15 +1211,12 @@
     <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.33203125" customWidth="1"/>
-    <col min="11" max="11" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="50.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="50.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="28.77734375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="27.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1263,14 +1314,26 @@
       <c r="K2" t="s">
         <v>64</v>
       </c>
+      <c r="L2" t="s">
+        <v>100</v>
+      </c>
       <c r="N2" t="s">
         <v>74</v>
       </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
       <c r="P2" t="s">
         <v>84</v>
       </c>
+      <c r="Q2" t="s">
+        <v>110</v>
+      </c>
       <c r="R2" t="s">
         <v>94</v>
+      </c>
+      <c r="S2" t="s">
+        <v>115</v>
       </c>
       <c r="T2" t="s">
         <v>15</v>
@@ -1327,11 +1390,20 @@
       <c r="K4" t="s">
         <v>65</v>
       </c>
+      <c r="L4" t="s">
+        <v>101</v>
+      </c>
       <c r="N4" t="s">
         <v>75</v>
       </c>
+      <c r="O4" t="s">
+        <v>106</v>
+      </c>
       <c r="P4" t="s">
         <v>85</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>111</v>
       </c>
       <c r="T4" t="s">
         <v>63</v>
@@ -1641,14 +1713,26 @@
       <c r="K14" t="s">
         <v>70</v>
       </c>
+      <c r="L14" t="s">
+        <v>102</v>
+      </c>
       <c r="N14" t="s">
         <v>80</v>
       </c>
+      <c r="O14" t="s">
+        <v>107</v>
+      </c>
       <c r="P14" t="s">
         <v>90</v>
       </c>
+      <c r="Q14" t="s">
+        <v>112</v>
+      </c>
       <c r="R14" t="s">
         <v>96</v>
+      </c>
+      <c r="S14" t="s">
+        <v>116</v>
       </c>
       <c r="T14" t="s">
         <v>41</v>
@@ -1705,11 +1789,20 @@
       <c r="K16" t="s">
         <v>71</v>
       </c>
+      <c r="L16" t="s">
+        <v>103</v>
+      </c>
       <c r="N16" t="s">
         <v>81</v>
       </c>
+      <c r="O16" t="s">
+        <v>108</v>
+      </c>
       <c r="P16" t="s">
         <v>91</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>113</v>
       </c>
       <c r="T16" t="s">
         <v>62</v>
@@ -1830,14 +1923,26 @@
       <c r="K20" t="s">
         <v>73</v>
       </c>
+      <c r="L20" t="s">
+        <v>104</v>
+      </c>
       <c r="N20" t="s">
         <v>83</v>
       </c>
+      <c r="O20" t="s">
+        <v>109</v>
+      </c>
       <c r="P20" t="s">
         <v>93</v>
       </c>
+      <c r="Q20" t="s">
+        <v>114</v>
+      </c>
       <c r="R20" t="s">
         <v>97</v>
+      </c>
+      <c r="S20" t="s">
+        <v>117</v>
       </c>
       <c r="T20" t="s">
         <v>58</v>

</xml_diff>